<commit_message>
fix overlapping bars for recon and retro (mostly)
</commit_message>
<xml_diff>
--- a/resources/data/profile_data_structure_template.xlsx
+++ b/resources/data/profile_data_structure_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Profile Data" sheetId="2" r:id="rId1"/>
@@ -3596,8 +3596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EQ40"/>
   <sheetViews>
-    <sheetView topLeftCell="CY3" workbookViewId="0">
-      <selection activeCell="DK4" sqref="DK4:DK16"/>
+    <sheetView tabSelected="1" topLeftCell="AN3" workbookViewId="0">
+      <selection activeCell="AX4" sqref="AX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4948,13 +4948,13 @@
         <v>5938</v>
       </c>
       <c r="AV4" s="6">
-        <v>5938</v>
+        <v>7000</v>
       </c>
       <c r="AW4" s="6">
-        <v>2634</v>
+        <v>6700</v>
       </c>
       <c r="AX4" s="6">
-        <v>1866</v>
+        <v>500</v>
       </c>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -12643,7 +12643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix m3 issue, trainings circle, Dec 15 issues
</commit_message>
<xml_diff>
--- a/resources/data/profile_data_structure_template.xlsx
+++ b/resources/data/profile_data_structure_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Profile Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="515">
   <si>
     <t>Facts and Figures</t>
   </si>
@@ -1561,9 +1561,6 @@
   </si>
   <si>
     <t>Affected by HEP</t>
-  </si>
-  <si>
-    <t>reached</t>
   </si>
   <si>
     <t>#value_en</t>
@@ -1661,8 +1658,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="293">
+  <cellStyleXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2019,7 +2020,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="293">
+  <cellStyles count="297">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2166,6 +2167,8 @@
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2312,6 +2315,8 @@
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3607,8 +3612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EQ40"/>
   <sheetViews>
-    <sheetView topLeftCell="DI1" workbookViewId="0">
-      <selection activeCell="DP5" sqref="DP5"/>
+    <sheetView tabSelected="1" topLeftCell="DT1" workbookViewId="0">
+      <selection activeCell="ED6" sqref="ED6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5420,8 +5425,7 @@
         <v>306</v>
       </c>
       <c r="ED5" s="11">
-        <f t="shared" ref="ED5:ED16" si="4">EB5-EC5</f>
-        <v>-45</v>
+        <v>45</v>
       </c>
       <c r="EE5" s="11">
         <v>378</v>
@@ -5430,7 +5434,7 @@
         <v>0</v>
       </c>
       <c r="EG5" s="11">
-        <f t="shared" ref="EG5:EG16" si="5">EE5-EF5</f>
+        <f t="shared" ref="EG5:EG16" si="4">EE5-EF5</f>
         <v>378</v>
       </c>
       <c r="EH5" s="6"/>
@@ -5705,7 +5709,7 @@
         <v>370</v>
       </c>
       <c r="ED6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="ED5:ED16" si="5">EB6-EC6</f>
         <v>47</v>
       </c>
       <c r="EE6" s="10">
@@ -5715,7 +5719,7 @@
         <v>8</v>
       </c>
       <c r="EG6" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>591</v>
       </c>
       <c r="EH6" s="6"/>
@@ -5980,7 +5984,7 @@
         <v>100</v>
       </c>
       <c r="ED7" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>296</v>
       </c>
       <c r="EE7" s="10">
@@ -5990,7 +5994,7 @@
         <v>6</v>
       </c>
       <c r="EG7" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>525</v>
       </c>
       <c r="EH7" s="6"/>
@@ -6239,7 +6243,7 @@
         <v>70</v>
       </c>
       <c r="ED8" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>287</v>
       </c>
       <c r="EE8" s="10">
@@ -6249,7 +6253,7 @@
         <v>90</v>
       </c>
       <c r="EG8" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>431</v>
       </c>
       <c r="EH8" s="6"/>
@@ -6506,7 +6510,7 @@
         <v>170</v>
       </c>
       <c r="ED9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="EE9" s="10">
@@ -6516,7 +6520,7 @@
         <v>24</v>
       </c>
       <c r="EG9" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="EH9" s="6"/>
@@ -6803,7 +6807,7 @@
         <v>36</v>
       </c>
       <c r="ED10" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="EE10" s="10">
@@ -6813,7 +6817,7 @@
         <v>190</v>
       </c>
       <c r="EG10" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="EH10" s="6"/>
@@ -7060,7 +7064,7 @@
         <v>402</v>
       </c>
       <c r="ED11" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>207</v>
       </c>
       <c r="EE11" s="10">
@@ -7070,7 +7074,7 @@
         <v>84</v>
       </c>
       <c r="EG11" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>802</v>
       </c>
       <c r="EH11" s="6"/>
@@ -7347,8 +7351,7 @@
         <v>674</v>
       </c>
       <c r="ED12" s="11">
-        <f t="shared" si="4"/>
-        <v>-203</v>
+        <v>203</v>
       </c>
       <c r="EE12" s="10">
         <v>666</v>
@@ -7357,7 +7360,7 @@
         <v>20</v>
       </c>
       <c r="EG12" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>646</v>
       </c>
       <c r="EH12" s="6"/>
@@ -7654,7 +7657,7 @@
         <v>460</v>
       </c>
       <c r="ED13" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="EE13" s="10">
@@ -7664,7 +7667,7 @@
         <v>0</v>
       </c>
       <c r="EG13" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>759</v>
       </c>
       <c r="EH13" s="6"/>
@@ -7921,7 +7924,7 @@
         <v>450</v>
       </c>
       <c r="ED14" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="EE14" s="10">
@@ -7931,7 +7934,7 @@
         <v>28</v>
       </c>
       <c r="EG14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>855</v>
       </c>
       <c r="EH14" s="6"/>
@@ -8172,7 +8175,7 @@
         <v>518</v>
       </c>
       <c r="ED15" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-122</v>
       </c>
       <c r="EE15" s="10">
@@ -8182,7 +8185,7 @@
         <v>38</v>
       </c>
       <c r="EG15" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>529</v>
       </c>
       <c r="EH15" s="6"/>
@@ -8435,7 +8438,7 @@
         <v>157</v>
       </c>
       <c r="ED16" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="EE16" s="10">
@@ -8445,7 +8448,7 @@
         <v>0</v>
       </c>
       <c r="EG16" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>432</v>
       </c>
       <c r="EH16" s="6"/>
@@ -8534,8 +8537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9554,10 +9557,10 @@
         <v>239</v>
       </c>
       <c r="E38" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -11265,7 +11268,7 @@
         <v>359</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G103" t="str">
         <f>INDEX([1]Titles!$G:$G,MATCH(A103,[1]Titles!$A:$A,0))</f>
@@ -11628,8 +11631,9 @@
         <f t="shared" si="9"/>
         <v>#training_vocational_training</v>
       </c>
-      <c r="B117" t="s">
-        <v>509</v>
+      <c r="B117" t="str">
+        <f t="shared" si="5"/>
+        <v>training_vocational_training</v>
       </c>
       <c r="C117">
         <f t="shared" si="8"/>
@@ -12682,10 +12686,10 @@
         <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12693,10 +12697,10 @@
         <v>225</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>